<commit_message>
added mycareerfuture job search
</commit_message>
<xml_diff>
--- a/KeywordLibrary_Comprehensive.xlsx
+++ b/KeywordLibrary_Comprehensive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff96ec12531e8c88/PBA/SCT5/Practicum/RPA-J-01  Job Matching for Placements/RPA-J-01 Job matching for Placements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Google Drive\Personal\UiPath\RPA-J-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{D01B27D8-D946-4ED6-B7CC-15EBC484F70D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3CDA7B6B-6BC5-4AD3-A836-6DEC057D48A9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66107E69-247D-466B-853B-7F3C02B387A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29535" yWindow="3660" windowWidth="14895" windowHeight="12435" xr2:uid="{4FC0F06C-D9D6-45DE-B83F-4A922B31FC97}"/>
+    <workbookView xWindow="12135" yWindow="2820" windowWidth="32280" windowHeight="15345" xr2:uid="{4FC0F06C-D9D6-45DE-B83F-4A922B31FC97}"/>
   </bookViews>
   <sheets>
     <sheet name="keyword" sheetId="1" r:id="rId1"/>
@@ -1956,14 +1956,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCB9B35-F431-45F4-8A59-C98B611EF534}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>